<commit_message>
remove a completely pointless reparse!
</commit_message>
<xml_diff>
--- a/Thousand.Benchmarks/baselines/summary.xlsx
+++ b/Thousand.Benchmarks/baselines/summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banana\Documents\code\thousand\Thousand.Benchmarks\baselines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9C5BEF9-A2AE-4CE2-B357-DBFCDD4EEB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8298E66E-A47D-4989-8E52-77D5E4F2458A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9150" yWindow="2715" windowWidth="28800" windowHeight="15435" xr2:uid="{E09EFE12-747D-4EEC-87FA-EF1C3FF6DC6E}"/>
   </bookViews>
@@ -199,10 +199,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:f>Sheet1!$B$2:$G$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>7.9290000000000003</c:v>
                 </c:pt>
@@ -217,6 +217,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6.7210000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.7359999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -256,10 +259,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$F$3</c:f>
+              <c:f>Sheet1!$B$3:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>7.6150000000000002</c:v>
                 </c:pt>
@@ -274,6 +277,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5.875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.8719999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -569,10 +575,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$M$2</c:f>
+              <c:f>Sheet1!$I$2:$N$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>15.507</c:v>
                 </c:pt>
@@ -587,6 +593,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>13.183999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -626,10 +635,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$3:$M$3</c:f>
+              <c:f>Sheet1!$I$3:$N$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>15.459</c:v>
                 </c:pt>
@@ -644,6 +653,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>12.561</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.631</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -939,10 +951,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$T$2</c:f>
+              <c:f>Sheet1!$P$2:$U$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>22.556000000000001</c:v>
                 </c:pt>
@@ -957,6 +969,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>19.949000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.010000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -996,10 +1011,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$3:$T$3</c:f>
+              <c:f>Sheet1!$P$3:$U$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>24.63</c:v>
                 </c:pt>
@@ -1014,6 +1029,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>19.510999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.853999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2900,7 +2918,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2936,8 +2954,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2968,14 +2986,14 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3302,10 +3320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7FF573F-EAF7-4AE9-8AC1-948A842A4C3C}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+      <selection activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3315,7 +3333,7 @@
     <col min="15" max="15" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3326,7 +3344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3345,6 +3363,9 @@
       <c r="F2">
         <v>6.7210000000000001</v>
       </c>
+      <c r="G2">
+        <v>5.7359999999999998</v>
+      </c>
       <c r="H2" t="s">
         <v>0</v>
       </c>
@@ -3363,6 +3384,9 @@
       <c r="M2">
         <v>13.183999999999999</v>
       </c>
+      <c r="N2">
+        <v>11.29</v>
+      </c>
       <c r="O2" t="s">
         <v>0</v>
       </c>
@@ -3381,8 +3405,11 @@
       <c r="T2">
         <v>19.949000000000002</v>
       </c>
+      <c r="U2">
+        <v>17.010000000000002</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3401,6 +3428,9 @@
       <c r="F3">
         <v>5.875</v>
       </c>
+      <c r="G3">
+        <v>4.8719999999999999</v>
+      </c>
       <c r="H3" t="s">
         <v>1</v>
       </c>
@@ -3419,6 +3449,9 @@
       <c r="M3">
         <v>12.561</v>
       </c>
+      <c r="N3">
+        <v>10.631</v>
+      </c>
       <c r="O3" t="s">
         <v>1</v>
       </c>
@@ -3436,6 +3469,9 @@
       </c>
       <c r="T3">
         <v>19.510999999999999</v>
+      </c>
+      <c r="U3">
+        <v>16.853999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>